<commit_message>
Exercise 2.1 and 2.3 are done
</commit_message>
<xml_diff>
--- a/assignment2/ass2exer2,3.xlsx
+++ b/assignment2/ass2exer2,3.xlsx
@@ -8,97 +8,219 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rinusvangrunsven/Documents/GitHub/SSO-group26/assignment2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB481ACB-B6A5-B14C-9038-2E990D98C247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6986531E-50DE-6D4E-A51C-F2221F4E3A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="500" windowWidth="27240" windowHeight="15940" activeTab="1" xr2:uid="{F0BFEBBF-DEC1-2547-8B31-F63FC2DC2A09}"/>
+    <workbookView xWindow="220" yWindow="500" windowWidth="27360" windowHeight="17120" activeTab="3" xr2:uid="{F0BFEBBF-DEC1-2547-8B31-F63FC2DC2A09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="a" sheetId="5" r:id="rId2"/>
+    <sheet name="b" sheetId="3" r:id="rId3"/>
+    <sheet name="c" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">a!$C$14:$G$14</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">b!$C$15:$H$15</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">'c'!$C$15:$G$15</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$C$12:$G$12</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">Sheet2!$C$13:$G$13</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">Sheet2!$C$13:$G$13</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">a!$I$6</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">b!$G$15</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'c'!$C$15:$G$15</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$I$5</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">Sheet2!$C$13:$G$13</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">Sheet2!$J$5</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">a!$I$7</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">b!$J$10</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'c'!$I$10</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$I$6</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">Sheet2!$J$5</definedName>
+    <definedName name="solver_lhs2" localSheetId="4" hidden="1">Sheet2!$J$6</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">a!$I$8</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">b!$J$7</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">'c'!$I$7</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$I$7</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">Sheet2!$J$6</definedName>
+    <definedName name="solver_lhs3" localSheetId="4" hidden="1">Sheet2!$J$7</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">a!$I$9</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">b!$J$8</definedName>
+    <definedName name="solver_lhs4" localSheetId="3" hidden="1">'c'!$I$8</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$I$8</definedName>
-    <definedName name="solver_lhs4" localSheetId="1" hidden="1">Sheet2!$J$7</definedName>
+    <definedName name="solver_lhs4" localSheetId="4" hidden="1">Sheet2!$J$8</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">b!$J$9</definedName>
+    <definedName name="solver_lhs5" localSheetId="3" hidden="1">'c'!$I$9</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">Sheet1!$I$8</definedName>
-    <definedName name="solver_lhs5" localSheetId="1" hidden="1">Sheet2!$J$8</definedName>
+    <definedName name="solver_lhs5" localSheetId="4" hidden="1">Sheet2!$J$8</definedName>
+    <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_lin" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
-    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
-    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">4</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">5</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">5</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">4</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">a!$C$22</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">'c'!$C$23</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$C$19</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">Sheet2!$C$21</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">Sheet2!$C$21</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
-    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">4</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel1" localSheetId="1" hidden="1">4</definedName>
+    <definedName name="solver_rel1" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel5" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">a!$K$6</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">5</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">"integer"</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">Sheet1!$K$5</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">"integer"</definedName>
+    <definedName name="solver_rhs1" localSheetId="4" hidden="1">Sheet2!$L$5</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">a!$K$7</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">b!$L$10</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">'c'!$K$10</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">Sheet1!$K$6</definedName>
-    <definedName name="solver_rhs2" localSheetId="1" hidden="1">Sheet2!$L$5</definedName>
+    <definedName name="solver_rhs2" localSheetId="4" hidden="1">Sheet2!$L$6</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">a!$K$8</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">b!$L$7</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">'c'!$K$7</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet1!$K$7</definedName>
-    <definedName name="solver_rhs3" localSheetId="1" hidden="1">Sheet2!$L$6</definedName>
+    <definedName name="solver_rhs3" localSheetId="4" hidden="1">Sheet2!$L$7</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">a!$K$9</definedName>
+    <definedName name="solver_rhs4" localSheetId="2" hidden="1">b!$L$8</definedName>
+    <definedName name="solver_rhs4" localSheetId="3" hidden="1">'c'!$K$8</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">Sheet1!$K$8</definedName>
-    <definedName name="solver_rhs4" localSheetId="1" hidden="1">Sheet2!$L$7</definedName>
+    <definedName name="solver_rhs4" localSheetId="4" hidden="1">Sheet2!$L$8</definedName>
+    <definedName name="solver_rhs5" localSheetId="2" hidden="1">b!$L$9</definedName>
+    <definedName name="solver_rhs5" localSheetId="3" hidden="1">'c'!$K$9</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">Sheet1!$K$8</definedName>
-    <definedName name="solver_rhs5" localSheetId="1" hidden="1">Sheet2!$L$8</definedName>
+    <definedName name="solver_rhs5" localSheetId="4" hidden="1">Sheet2!$L$8</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
-    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -120,7 +242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="46">
   <si>
     <t>Constraints</t>
   </si>
@@ -264,7 +386,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -282,6 +404,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -331,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -351,6 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1248,11 +1378,948 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AAA8D6F-D4F9-E74B-A5B8-C58291AF1913}">
+  <dimension ref="B4:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>171</v>
+      </c>
+      <c r="E6">
+        <v>65</v>
+      </c>
+      <c r="F6">
+        <v>112</v>
+      </c>
+      <c r="G6">
+        <v>188</v>
+      </c>
+      <c r="I6">
+        <f>SUMPRODUCT(C6:G6,C18:G18)</f>
+        <v>3063.8416930166732</v>
+      </c>
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>0.1</v>
+      </c>
+      <c r="D7">
+        <v>0.2</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G7">
+        <v>16</v>
+      </c>
+      <c r="I7">
+        <f>SUMPRODUCT(C7:G7,C18:G18)</f>
+        <v>150.02236239539383</v>
+      </c>
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>0.6</v>
+      </c>
+      <c r="D8">
+        <v>3.7</v>
+      </c>
+      <c r="E8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>7.7</v>
+      </c>
+      <c r="I8">
+        <f>SUMPRODUCT(C8:G8,C18:G18)</f>
+        <v>100.0000004829234</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>30</v>
+      </c>
+      <c r="E9">
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <f>SUMPRODUCT(C9:G9,C18:G18)</f>
+        <v>250</v>
+      </c>
+      <c r="J9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.12</v>
+      </c>
+      <c r="E10">
+        <v>0.2</v>
+      </c>
+      <c r="F10">
+        <v>0.75</v>
+      </c>
+      <c r="G10">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>7.7146690475588251</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>9.2799642866176288</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <f>C14</f>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:G18" si="0">D14</f>
+        <v>7.7146690475588251</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>9.2799642866176288</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D19">
+        <v>0.12</v>
+      </c>
+      <c r="E19">
+        <v>0.2</v>
+      </c>
+      <c r="F19">
+        <v>0.75</v>
+      </c>
+      <c r="G19">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>3.6720000000000002</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <f>SUMPRODUCT(C18:G18,C19:G19)</f>
+        <v>2.3177549286997032</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8AF7C6-FE17-A84F-A4C4-D0A6EEA37715}">
+  <dimension ref="B3:L23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>171</v>
+      </c>
+      <c r="E7">
+        <v>65</v>
+      </c>
+      <c r="F7">
+        <v>112</v>
+      </c>
+      <c r="G7">
+        <v>188</v>
+      </c>
+      <c r="H7">
+        <v>188</v>
+      </c>
+      <c r="J7">
+        <f>SUMPRODUCT(C7:H7,C19:H19)</f>
+        <v>3782.2973259544938</v>
+      </c>
+      <c r="K7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>0.1</v>
+      </c>
+      <c r="D8">
+        <v>0.2</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G8">
+        <v>16</v>
+      </c>
+      <c r="H8">
+        <v>16</v>
+      </c>
+      <c r="J8">
+        <f>SUMPRODUCT(C8:H8,C19:H19)</f>
+        <v>83.324324357841519</v>
+      </c>
+      <c r="K8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>0.6</v>
+      </c>
+      <c r="D9">
+        <v>3.7</v>
+      </c>
+      <c r="E9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>7.7</v>
+      </c>
+      <c r="H9">
+        <v>7.7</v>
+      </c>
+      <c r="J9">
+        <f>SUMPRODUCT(C9:H9,C19:H19)</f>
+        <v>100.00000062006799</v>
+      </c>
+      <c r="K9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>30</v>
+      </c>
+      <c r="E10">
+        <v>13</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <f>SUMPRODUCT(C10:H10,C19:H19)</f>
+        <v>508.64865367622701</v>
+      </c>
+      <c r="K10" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D11">
+        <v>0.12</v>
+      </c>
+      <c r="E11">
+        <v>0.2</v>
+      </c>
+      <c r="F11">
+        <v>0.75</v>
+      </c>
+      <c r="G11">
+        <v>0.15</v>
+      </c>
+      <c r="H11">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>16.621621789207566</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <f>C15</f>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:G19" si="0">D15</f>
+        <v>16.621621789207566</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <f>H15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.12</v>
+      </c>
+      <c r="E20">
+        <v>0.2</v>
+      </c>
+      <c r="F20">
+        <v>0.75</v>
+      </c>
+      <c r="G20">
+        <v>0.15</v>
+      </c>
+      <c r="H20">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>3.6720000000000002</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0.75</v>
+      </c>
+      <c r="H21">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23">
+        <f>SUMPRODUCT(C19:H19,C20:H20)</f>
+        <v>2.7445946147049076</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B58775-F5C5-7B47-B729-7426723DB05B}">
+  <dimension ref="B5:K23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>171</v>
+      </c>
+      <c r="E7">
+        <v>65</v>
+      </c>
+      <c r="F7">
+        <v>112</v>
+      </c>
+      <c r="G7">
+        <v>188</v>
+      </c>
+      <c r="I7">
+        <f>SUMPRODUCT(C7:G7,C19:G19)</f>
+        <v>3231</v>
+      </c>
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>0.1</v>
+      </c>
+      <c r="D8">
+        <v>0.2</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G8">
+        <v>16</v>
+      </c>
+      <c r="I8">
+        <f>SUMPRODUCT(C8:G8,C19:G19)</f>
+        <v>145.80000000000001</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>0.6</v>
+      </c>
+      <c r="D9">
+        <v>3.7</v>
+      </c>
+      <c r="E9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>7.7</v>
+      </c>
+      <c r="I9">
+        <f>SUMPRODUCT(C9:G9,C19:G19)</f>
+        <v>102.6</v>
+      </c>
+      <c r="J9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>30</v>
+      </c>
+      <c r="E10">
+        <v>13</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <f>SUMPRODUCT(C10:G10,C19:G19)</f>
+        <v>288</v>
+      </c>
+      <c r="J10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D11">
+        <v>0.12</v>
+      </c>
+      <c r="E11">
+        <v>0.2</v>
+      </c>
+      <c r="F11">
+        <v>0.75</v>
+      </c>
+      <c r="G11">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <f>C15</f>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f>D15</f>
+        <v>9</v>
+      </c>
+      <c r="E19">
+        <f>E15</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f>F15</f>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f>G15</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.12</v>
+      </c>
+      <c r="E20">
+        <v>0.2</v>
+      </c>
+      <c r="F20">
+        <v>0.75</v>
+      </c>
+      <c r="G20">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>3.6720000000000002</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23">
+        <f>SUMPRODUCT(C19:G19,C20:G20)</f>
+        <v>2.4299999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A654BFED-C4E5-9642-8330-9B2DA4C52C88}">
   <dimension ref="B3:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>